<commit_message>
add missing cervicalcancer book
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_cervicalcancer.xlsx
+++ b/tests/databooks/databook_cervicalcancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60E8E753-9D9F-3B40-AC30-BA305EEAEDBE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A7CC0AAC-A750-FC47-A189-A5EB2FED8BDA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,6 +26,39 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{845BC4E9-381F-9148-9E7A-6C2F2512240A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F5" authorId="0" shapeId="0" xr:uid="{8853CF8D-7FF1-1842-8E56-1BFE3493BA6C}">
       <text>
         <r>
@@ -55,16 +88,40 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Assuming prevalence of 0.5%, taken from a study in Nigeria - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
+          <t>Assuming prevalence of 0.5%, taken from a study in Nigeria - https://www.ncbi.nlm.nih.gov/pubmed/29479954</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{5E306F34-DD0F-464D-A60F-0C8C001FEFF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
         </r>
       </text>
     </comment>
@@ -96,9 +153,41 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>9.3% (All women aged 15-49 ever screened, DHS 2010 Armenia)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{A627974C-8C27-5A48-BA2F-C2619CFBFEBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assume that 80% of those with cervical cancer who received a screening were diagnosed with cervical cancer</t>
         </r>
       </text>
     </comment>
@@ -135,6 +224,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{9675F3D2-A632-3041-94C7-1F6E14855256}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assume 50% are treated</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F14" authorId="0" shapeId="0" xr:uid="{DC2C1505-DF38-2F42-A5A1-188C166B452A}">
       <text>
         <r>
@@ -165,6 +287,48 @@
             <family val="2"/>
           </rPr>
           <t>Assume 50% are treated</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{F0289E20-6DD0-E141-A304-BC6BD34C2399}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">From </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
         </r>
       </text>
     </comment>
@@ -197,16 +361,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">From </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
+          <t>From http://www.hpvcentre.net/statistics/reports/ARM.pdf</t>
         </r>
       </text>
     </comment>
@@ -250,9 +405,6 @@
     <t>Annual number newly initiated onto treatment</t>
   </si>
   <si>
-    <t>Annual number lost to follow-up</t>
-  </si>
-  <si>
     <t>Mortality rate</t>
   </si>
   <si>
@@ -278,6 +430,9 @@
   </si>
   <si>
     <t>Estimated number of women with cervical cancer who have ever been diagnosed</t>
+  </si>
+  <si>
+    <t>Mortality rate for those with untreated cervical cancer</t>
   </si>
 </sst>
 </file>
@@ -318,7 +473,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -399,7 +553,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp"/>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -902,10 +1068,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -920,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -968,7 +1134,10 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <f>F2/1.01</f>
+        <v>636340.59405940596</v>
+      </c>
       <c r="F2" s="2">
         <v>642704</v>
       </c>
@@ -977,7 +1146,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1011,7 +1180,10 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <f>5/1000*E2</f>
+        <v>3181.7029702970299</v>
+      </c>
       <c r="F5" s="2">
         <f>5/1000*F2</f>
         <v>3213.52</v>
@@ -1021,7 +1193,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1055,7 +1227,10 @@
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <f>E5*0.093</f>
+        <v>295.89837623762378</v>
+      </c>
       <c r="F8" s="2">
         <f>F5*0.093</f>
         <v>298.85735999999997</v>
@@ -1065,7 +1240,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -1099,7 +1274,10 @@
       <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <f>E8*0.9</f>
+        <v>266.3085386138614</v>
+      </c>
       <c r="F11" s="2">
         <f>F8*0.9</f>
         <v>268.97162399999996</v>
@@ -1109,7 +1287,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -1143,7 +1321,10 @@
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <f>E11*0.5</f>
+        <v>133.1542693069307</v>
+      </c>
       <c r="F14" s="2">
         <f>F11*0.5</f>
         <v>134.48581199999998</v>
@@ -1187,7 +1368,10 @@
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <f>13/1000*E2</f>
+        <v>8272.4277227722778</v>
+      </c>
       <c r="F17" s="2">
         <f>13/1000*F2</f>
         <v>8355.152</v>
@@ -1197,7 +1381,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -1231,7 +1415,9 @@
       <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>272</v>
+      </c>
       <c r="F20" s="2">
         <v>272</v>
       </c>
@@ -1274,7 +1460,10 @@
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <f>0.093*E2</f>
+        <v>59179.675247524756</v>
+      </c>
       <c r="F23" s="2">
         <f>0.093*F2</f>
         <v>59771.472000000002</v>
@@ -1318,7 +1507,10 @@
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2">
+        <f>200</f>
+        <v>200</v>
+      </c>
       <c r="F26" s="2">
         <f>200</f>
         <v>200</v>
@@ -1362,7 +1554,9 @@
       <c r="D29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>80</v>
+      </c>
       <c r="F29" s="2">
         <v>80</v>
       </c>
@@ -1399,22 +1593,22 @@
         <v>women</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2">
-        <v>20</v>
-      </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
@@ -1442,10 +1636,10 @@
         <v>women</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>6</v>
@@ -1457,106 +1651,106 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="24" priority="10">
       <formula>AND(COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="23" priority="11">
       <formula>COUNTIF(E14:H14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="22" priority="12">
       <formula>AND(COUNTIF(E14:H14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="21" priority="13">
       <formula>COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="20" priority="14">
       <formula>AND(COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>AND(COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>AND(COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>AND(COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="11" priority="17">
+    <cfRule type="expression" dxfId="13" priority="19">
       <formula>COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="18">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>AND(COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="9" priority="19">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>COUNTIF(E29:H29,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="20">
+    <cfRule type="expression" dxfId="10" priority="22">
       <formula>AND(COUNTIF(E29:H29,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="7" priority="21">
+    <cfRule type="expression" dxfId="7" priority="25">
       <formula>COUNTIF(E32:H32,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="22">
+    <cfRule type="expression" dxfId="6" priority="26">
       <formula>AND(COUNTIF(E32:H32,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>COUNTIF(E8:H8,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>AND(COUNTIF(E8:H8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="5" priority="23">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>COUNTIF(E35:H35,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="24">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>AND(COUNTIF(E35:H35,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="1" priority="5">
-      <formula>COUNTIF(E8:H8,"&lt;&gt;" &amp; "")&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(COUNTIF(E8:H8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B32 B29 B26 B23 B20 B17 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B29 B26 B23 B20 B17 B14 B11 B8 B5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32 B35" xr:uid="{00000000-0002-0000-0100-00000B000000}">
       <formula1>"Probability"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>